<commit_message>
changes to example files
</commit_message>
<xml_diff>
--- a/python/examples/example_data/excel_spreadsheet_files/input.xlsx
+++ b/python/examples/example_data/excel_spreadsheet_files/input.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/weymouth/Dropbox/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/weymouth/workspace/src/github.com/materials-commons/mcapi/python/examples/example_data/excel_spreadsheet_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="41">
   <si>
     <t>action</t>
   </si>
@@ -141,6 +141,15 @@
   </si>
   <si>
     <t>Sectioning B</t>
+  </si>
+  <si>
+    <t>Analysis</t>
+  </si>
+  <si>
+    <t>Computation</t>
+  </si>
+  <si>
+    <t>[SampleB2,SampleA2]</t>
   </si>
 </sst>
 </file>
@@ -455,10 +464,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I16"/>
+  <dimension ref="A1:I17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -466,6 +475,9 @@
     <col min="2" max="2" width="16.6640625" customWidth="1"/>
     <col min="3" max="3" width="21.1640625" customWidth="1"/>
     <col min="4" max="4" width="21.83203125" customWidth="1"/>
+    <col min="5" max="5" width="28.5" customWidth="1"/>
+    <col min="6" max="6" width="24.33203125" customWidth="1"/>
+    <col min="7" max="7" width="18" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.2">
@@ -678,6 +690,17 @@
         <v>30</v>
       </c>
     </row>
+    <row r="17" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B17" t="s">
+        <v>38</v>
+      </c>
+      <c r="D17" t="s">
+        <v>39</v>
+      </c>
+      <c r="E17" t="s">
+        <v>40</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Data for examples; update spreadsheet
</commit_message>
<xml_diff>
--- a/python/examples/example_data/excel_spreadsheet_files/input.xlsx
+++ b/python/examples/example_data/excel_spreadsheet_files/input.xlsx
@@ -92,9 +92,6 @@
     <t>SEM</t>
   </si>
   <si>
-    <t>SEM1_data</t>
-  </si>
-  <si>
     <t>SampleA1</t>
   </si>
   <si>
@@ -104,12 +101,6 @@
     <t>Fatigue</t>
   </si>
   <si>
-    <t>Fatigue_data</t>
-  </si>
-  <si>
-    <t>SEM2_data</t>
-  </si>
-  <si>
     <t>Sample B</t>
   </si>
   <si>
@@ -150,6 +141,15 @@
   </si>
   <si>
     <t>[SampleB2,SampleA2]</t>
+  </si>
+  <si>
+    <t>SEM1_Data</t>
+  </si>
+  <si>
+    <t>Fatigue_Data</t>
+  </si>
+  <si>
+    <t>SEM2_Data</t>
   </si>
 </sst>
 </file>
@@ -466,8 +466,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -503,7 +503,7 @@
         <v>12</v>
       </c>
       <c r="H1" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="I1" t="s">
         <v>8</v>
@@ -517,7 +517,7 @@
         <v>4</v>
       </c>
       <c r="C3" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
@@ -545,7 +545,7 @@
         <v>15</v>
       </c>
       <c r="H5" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
@@ -567,10 +567,10 @@
         <v>19</v>
       </c>
       <c r="D7" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="E7" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
@@ -581,10 +581,10 @@
         <v>20</v>
       </c>
       <c r="E8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G8" t="s">
-        <v>21</v>
+        <v>38</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
@@ -592,27 +592,27 @@
         <v>19</v>
       </c>
       <c r="D9" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="E9" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H9" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B10" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D10" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="E10" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G10" t="s">
-        <v>25</v>
+        <v>39</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.2">
@@ -623,10 +623,10 @@
         <v>20</v>
       </c>
       <c r="E11" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G11" t="s">
-        <v>26</v>
+        <v>40</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.2">
@@ -634,27 +634,27 @@
         <v>13</v>
       </c>
       <c r="B12" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="D12" t="s">
         <v>14</v>
       </c>
       <c r="F12" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B13" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="D13" t="s">
         <v>17</v>
       </c>
       <c r="E13" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="F13" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.2">
@@ -665,18 +665,18 @@
         <v>20</v>
       </c>
       <c r="E14" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B15" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D15" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="E15" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.2">
@@ -687,18 +687,18 @@
         <v>20</v>
       </c>
       <c r="E16" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
     </row>
     <row r="17" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B17" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="D17" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="E17" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
   </sheetData>

</xml_diff>